<commit_message>
complete My Address module
</commit_message>
<xml_diff>
--- a/src/test/java/com/mystore/testData/AuthenticationModuleData.xlsx
+++ b/src/test/java/com/mystore/testData/AuthenticationModuleData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EmailCheckData" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="CustomerInfoData" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="SignInData" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="ResetEmailData" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="UpdateCustomerData" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="59">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -170,6 +171,36 @@
   </si>
   <si>
     <t xml:space="preserve">sdewrwr@diu.edu.bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acharja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adfdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adfdfqw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdfdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdfdA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dshsjd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgbsf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfdsfds</t>
   </si>
 </sst>
 </file>
@@ -272,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +344,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +421,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -949,7 +984,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.68"/>
@@ -1013,11 +1048,11 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.47"/>
   </cols>
@@ -1052,4 +1087,280 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>1912</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>19121514</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete Automation for ContactUsModule using DDF
</commit_message>
<xml_diff>
--- a/src/test/java/com/mystore/testData/AuthenticationModuleData.xlsx
+++ b/src/test/java/com/mystore/testData/AuthenticationModuleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EmailCheckData" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr</t>
+    <t xml:space="preserve">Mr.</t>
   </si>
   <si>
     <t xml:space="preserve">ABC</t>
@@ -107,9 +107,6 @@
     <t xml:space="preserve">DEF</t>
   </si>
   <si>
-    <t xml:space="preserve">sdsdfeer@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">May </t>
   </si>
   <si>
@@ -146,16 +143,22 @@
     <t xml:space="preserve">dfdfdfdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrs</t>
+    <t xml:space="preserve">Mrs.</t>
   </si>
   <si>
     <t xml:space="preserve">!@@#$%</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEF123</t>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCiuy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deouoif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!@$%^&amp;</t>
   </si>
   <si>
     <t xml:space="preserve">cvcdvfdf64564636@gmail.com</t>
@@ -303,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -332,8 +335,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -418,20 +425,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -445,57 +451,54 @@
         <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -509,26 +512,26 @@
       <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4" t="n">
+        <v>1234</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>1234</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>29</v>
@@ -539,29 +542,26 @@
       <c r="M2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="n">
+        <v>19123</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="4" t="n">
-        <v>19123</v>
-      </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="S2" s="4" t="n">
-        <v>54587148</v>
-      </c>
-      <c r="T2" s="4" t="n">
-        <v>8978545212</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -574,26 +574,26 @@
       <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>29</v>
@@ -604,34 +604,31 @@
       <c r="M3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>25</v>
@@ -639,26 +636,26 @@
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>29</v>
@@ -669,34 +666,31 @@
       <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="R4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>25</v>
@@ -704,26 +698,26 @@
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H5" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>29</v>
@@ -734,34 +728,31 @@
       <c r="M5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="n">
+        <v>1912</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="4" t="n">
-        <v>1912</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="S5" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="T5" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="S5" s="4" t="n">
-        <v>54587148</v>
-      </c>
-      <c r="T5" s="4" t="n">
-        <v>8978545212</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>25</v>
@@ -769,26 +760,26 @@
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>29</v>
@@ -799,69 +790,69 @@
       <c r="M6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="4" t="n">
+        <v>191212</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="4" t="n">
-        <v>191212</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>54587148</v>
-      </c>
-      <c r="T6" s="4" t="n">
-        <v>8978545212</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="n">
+      <c r="E7" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="4" t="n">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="4" t="n">
         <v>54587148</v>
       </c>
+      <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
@@ -873,26 +864,26 @@
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>1998</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>29</v>
@@ -903,66 +894,186 @@
       <c r="M8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="4" t="n">
+        <v>19121</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="4" t="n">
+      <c r="Q8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>243546</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>45645</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>243546</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>45645</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="4" t="n">
         <v>19121</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="P9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R9" s="4" t="n">
+        <v>54587148</v>
+      </c>
+      <c r="S9" s="4" t="n">
+        <v>8978545212</v>
+      </c>
+      <c r="T9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S8" s="4" t="n">
+    </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="4" t="n">
+        <v>19121</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="4" t="n">
         <v>54587148</v>
       </c>
-      <c r="T8" s="4" t="n">
+      <c r="S10" s="4" t="n">
         <v>8978545212</v>
       </c>
-      <c r="U8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="8"/>
+      <c r="T10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="9"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="sdsdfeer@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="sdsdfeer@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="sdsdfeer@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="sdsdfeer@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="sdsdfeer@gmail.com"/>
-    <hyperlink ref="D8" r:id="rId6" display="sdsdfeer@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -984,7 +1095,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.68"/>
@@ -999,31 +1110,31 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="9" t="n">
+      <c r="A2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="10" t="n">
         <v>45689952</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="9" t="n">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="10" t="n">
         <v>12345</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>46</v>
+      <c r="B5" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1163,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.47"/>
   </cols>
@@ -1063,17 +1174,17 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>47</v>
+      <c r="A2" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>48</v>
+      <c r="A3" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1096,11 +1207,11 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.23"/>
@@ -1154,34 +1265,34 @@
     </row>
     <row r="2" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>1912</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="K2" s="4" t="n">
         <v>54587148</v>
@@ -1190,39 +1301,39 @@
         <v>8978545212</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>19121514</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="K3" s="4" t="n">
         <v>54587148</v>
@@ -1231,7 +1342,7 @@
         <v>8978545212</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1242,37 +1353,37 @@
         <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1283,75 +1394,75 @@
         <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="s">
         <v>58</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>